<commit_message>
add product to cart
</commit_message>
<xml_diff>
--- a/TEMPS/database-ecommerce.xlsx
+++ b/TEMPS/database-ecommerce.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Django\mysite\TEMPS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\Python\mysite\TEMPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3EC7679-F715-4FF3-A240-847A7695C214}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3387E7FB-E4C0-487E-864F-5F6D1991584A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" xr2:uid="{95E6102E-BFE5-48CA-B125-283D6CE05FC7}"/>
   </bookViews>
@@ -1129,15 +1129,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>42862</xdr:colOff>
+      <xdr:colOff>4762</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>923924</xdr:colOff>
+      <xdr:colOff>885824</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>61913</xdr:rowOff>
+      <xdr:rowOff>71438</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1152,8 +1152,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000" flipH="1">
-          <a:off x="8924924" y="3719513"/>
-          <a:ext cx="1185863" cy="1119187"/>
+          <a:off x="8882062" y="3733800"/>
+          <a:ext cx="1195388" cy="1119187"/>
         </a:xfrm>
         <a:prstGeom prst="bentArrow">
           <a:avLst/>
@@ -1247,7 +1247,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1545,8 +1545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A06BE9-8163-4315-8404-44365A89419E}">
   <dimension ref="B1:X33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X11" sqref="X11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>